<commit_message>
Respond to PR comments
</commit_message>
<xml_diff>
--- a/template_examples/nanostring_template.xlsx
+++ b/template_examples/nanostring_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="olink" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="nanostring" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="raw data" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Legend" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Data Dictionary" sheetId="4" state="visible" r:id="rId5"/>
@@ -601,11 +601,11 @@
   </sheetPr>
   <dimension ref="A1:C2009"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -10735,11 +10735,11 @@
   </sheetPr>
   <dimension ref="A1:D2005"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -20843,7 +20843,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
@@ -21034,7 +21034,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>

</xml_diff>